<commit_message>
Modified Structure to Run from SMIP/Main.py
By restructuring the project we are now able to run the application from the terminal by going into the SMIP directory and then running python3 Main.py
</commit_message>
<xml_diff>
--- a/grading/Another One(Grades).xlsx
+++ b/grading/Another One(Grades).xlsx
@@ -576,10 +576,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>2147482344</v>
+        <v>2147482380</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>2147482348</v>
+        <v>2147482384</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>0</v>
@@ -648,7 +648,7 @@
         <v>268468224</v>
       </c>
       <c r="AF2" s="2" t="n">
-        <v>2147482340</v>
+        <v>2147482376</v>
       </c>
       <c r="AG2" s="2" t="n">
         <v>0</v>
@@ -684,10 +684,10 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>2147482344</v>
+        <v>2147482380</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>2147482348</v>
+        <v>2147482384</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>0</v>
@@ -756,7 +756,7 @@
         <v>268468224</v>
       </c>
       <c r="AF3" s="2" t="n">
-        <v>2147482340</v>
+        <v>2147482376</v>
       </c>
       <c r="AG3" s="2" t="n">
         <v>0</v>
@@ -792,10 +792,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>2147482344</v>
+        <v>2147482380</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>2147482348</v>
+        <v>2147482384</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>0</v>
@@ -864,7 +864,7 @@
         <v>268468224</v>
       </c>
       <c r="AF4" s="2" t="n">
-        <v>2147482340</v>
+        <v>2147482376</v>
       </c>
       <c r="AG4" s="2" t="n">
         <v>0</v>
@@ -900,10 +900,10 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>2147482344</v>
+        <v>2147482380</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>2147482348</v>
+        <v>2147482384</v>
       </c>
       <c r="J5" s="2" t="n">
         <v>0</v>
@@ -972,7 +972,7 @@
         <v>268468224</v>
       </c>
       <c r="AF5" s="2" t="n">
-        <v>2147482340</v>
+        <v>2147482376</v>
       </c>
       <c r="AG5" s="2" t="n">
         <v>0</v>
@@ -1008,10 +1008,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>2147482344</v>
+        <v>2147482380</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>2147482348</v>
+        <v>2147482384</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>0</v>
@@ -1080,7 +1080,7 @@
         <v>268468224</v>
       </c>
       <c r="AF6" s="2" t="n">
-        <v>2147482340</v>
+        <v>2147482376</v>
       </c>
       <c r="AG6" s="2" t="n">
         <v>0</v>
@@ -1116,10 +1116,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>2147482344</v>
+        <v>2147482380</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>2147482348</v>
+        <v>2147482384</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>0</v>
@@ -1188,7 +1188,7 @@
         <v>268468224</v>
       </c>
       <c r="AF7" s="2" t="n">
-        <v>2147482340</v>
+        <v>2147482376</v>
       </c>
       <c r="AG7" s="2" t="n">
         <v>0</v>
@@ -1224,10 +1224,10 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>2147482344</v>
+        <v>2147482380</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>2147482348</v>
+        <v>2147482384</v>
       </c>
       <c r="J8" s="2" t="n">
         <v>0</v>
@@ -1296,7 +1296,7 @@
         <v>268468224</v>
       </c>
       <c r="AF8" s="2" t="n">
-        <v>2147482340</v>
+        <v>2147482376</v>
       </c>
       <c r="AG8" s="2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Major code restyle and import cleanup & Ran all Acceptance Tests
Used Black python reformatter to reformat entire projects code and make it cleaner. Cleaned up imports by removing unused imports and not using * imports. Confirmed all Acceptance Tests pass.
</commit_message>
<xml_diff>
--- a/grading/Another One(Grades).xlsx
+++ b/grading/Another One(Grades).xlsx
@@ -576,10 +576,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>2147482380</v>
+        <v>2147482232</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>2147482384</v>
+        <v>2147482236</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>0</v>
@@ -648,7 +648,7 @@
         <v>268468224</v>
       </c>
       <c r="AF2" s="2" t="n">
-        <v>2147482376</v>
+        <v>2147482228</v>
       </c>
       <c r="AG2" s="2" t="n">
         <v>0</v>
@@ -684,10 +684,10 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>2147482380</v>
+        <v>2147482232</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>2147482384</v>
+        <v>2147482236</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>0</v>
@@ -756,7 +756,7 @@
         <v>268468224</v>
       </c>
       <c r="AF3" s="2" t="n">
-        <v>2147482376</v>
+        <v>2147482228</v>
       </c>
       <c r="AG3" s="2" t="n">
         <v>0</v>
@@ -792,10 +792,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>2147482380</v>
+        <v>2147482232</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>2147482384</v>
+        <v>2147482236</v>
       </c>
       <c r="J4" s="2" t="n">
         <v>0</v>
@@ -864,7 +864,7 @@
         <v>268468224</v>
       </c>
       <c r="AF4" s="2" t="n">
-        <v>2147482376</v>
+        <v>2147482228</v>
       </c>
       <c r="AG4" s="2" t="n">
         <v>0</v>
@@ -900,10 +900,10 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>2147482380</v>
+        <v>2147482232</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>2147482384</v>
+        <v>2147482236</v>
       </c>
       <c r="J5" s="2" t="n">
         <v>0</v>
@@ -972,7 +972,7 @@
         <v>268468224</v>
       </c>
       <c r="AF5" s="2" t="n">
-        <v>2147482376</v>
+        <v>2147482228</v>
       </c>
       <c r="AG5" s="2" t="n">
         <v>0</v>
@@ -1008,10 +1008,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>2147482380</v>
+        <v>2147482232</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>2147482384</v>
+        <v>2147482236</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>0</v>
@@ -1080,7 +1080,7 @@
         <v>268468224</v>
       </c>
       <c r="AF6" s="2" t="n">
-        <v>2147482376</v>
+        <v>2147482228</v>
       </c>
       <c r="AG6" s="2" t="n">
         <v>0</v>
@@ -1116,10 +1116,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>2147482380</v>
+        <v>2147482232</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>2147482384</v>
+        <v>2147482236</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>0</v>
@@ -1188,7 +1188,7 @@
         <v>268468224</v>
       </c>
       <c r="AF7" s="2" t="n">
-        <v>2147482376</v>
+        <v>2147482228</v>
       </c>
       <c r="AG7" s="2" t="n">
         <v>0</v>
@@ -1224,10 +1224,10 @@
         <v>0</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>2147482380</v>
+        <v>2147482232</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>2147482384</v>
+        <v>2147482236</v>
       </c>
       <c r="J8" s="2" t="n">
         <v>0</v>
@@ -1296,7 +1296,7 @@
         <v>268468224</v>
       </c>
       <c r="AF8" s="2" t="n">
-        <v>2147482376</v>
+        <v>2147482228</v>
       </c>
       <c r="AG8" s="2" t="n">
         <v>0</v>

</xml_diff>